<commit_message>
adicionado tratativa para numeros invalidos
</commit_message>
<xml_diff>
--- a/envioWhatsapp.xlsx
+++ b/envioWhatsapp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projetos\AMC\envioWhatsapp\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB947B98-F423-464A-9E5E-2C7EB16908B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDA5E54D-9C2D-494D-96D9-2B53623D9D23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2520" yWindow="1035" windowWidth="25635" windowHeight="14445" xr2:uid="{7AA9F549-6323-4C7C-A194-0B25DA7E5875}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Telefone</t>
   </si>
@@ -409,15 +409,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45769F5C-D547-4B68-A325-B26E6E70AB58}">
-  <dimension ref="A1:F2"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" customWidth="1"/>
     <col min="5" max="5" width="120.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="46.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -438,7 +438,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>47988021117</v>
+        <v>4798802111777</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
@@ -448,6 +448,14 @@
       </c>
       <c r="F2" s="1" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>47988021117</v>
+      </c>
+      <c r="B3" t="s">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>